<commit_message>
updates to temperature table
</commit_message>
<xml_diff>
--- a/figure/Temperature Table.xlsx
+++ b/figure/Temperature Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14360" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14260" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="70">
   <si>
     <t xml:space="preserve">This should be a used as a literature reference for formulating FSI </t>
   </si>
@@ -195,9 +195,6 @@
     </r>
   </si>
   <si>
-    <t>Lenz16</t>
-  </si>
-  <si>
     <t xml:space="preserve">Schwartz93 </t>
   </si>
   <si>
@@ -235,6 +232,30 @@
   </si>
   <si>
     <t>extra notes</t>
+  </si>
+  <si>
+    <t>DVR</t>
+  </si>
+  <si>
+    <t>Sorbus aucuparia</t>
+  </si>
+  <si>
+    <t>Prunus avium</t>
+  </si>
+  <si>
+    <t>Tilia platyphyllos</t>
+  </si>
+  <si>
+    <t>Acer pseudoplatanus</t>
+  </si>
+  <si>
+    <t>Fagus sylvatica</t>
+  </si>
+  <si>
+    <t>LT50</t>
+  </si>
+  <si>
+    <t>Lenz16, Lenz13</t>
   </si>
 </sst>
 </file>
@@ -291,8 +312,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -301,11 +332,21 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -573,7 +614,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -670,7 +711,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
         <v>45</v>
@@ -686,10 +727,10 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
         <v>61</v>
-      </c>
-      <c r="B22" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -856,7 +897,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -871,15 +912,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -896,7 +939,7 @@
         <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F1" t="s">
         <v>46</v>
@@ -904,52 +947,144 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2">
+        <v>-7.4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>68</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
       </c>
       <c r="D3">
-        <v>-2.2000000000000002</v>
+        <v>-8.5</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
       </c>
       <c r="D4">
-        <v>-1.7</v>
+        <v>-7.4</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5">
+        <v>-6.7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6">
+        <v>-4.8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="E7" t="s">
         <v>51</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>-1.7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
         <v>58</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -980,17 +1115,17 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated temperature table, first rough draft
</commit_message>
<xml_diff>
--- a/figure/Temperature Table.xlsx
+++ b/figure/Temperature Table.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CatherineChamberlain/Documents/git/springfreeze/figure/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14260" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -15,18 +20,18 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="124">
   <si>
     <t xml:space="preserve">This should be a used as a literature reference for formulating FSI </t>
   </si>
@@ -195,9 +200,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Schwartz93 </t>
-  </si>
-  <si>
     <t>Ecology</t>
   </si>
   <si>
@@ -219,12 +221,6 @@
     <t>MSU ANR</t>
   </si>
   <si>
-    <t>2 or more days at 2 Standard Deviations below the Average Winter Temperature</t>
-  </si>
-  <si>
-    <t>Vavrus06</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -234,9 +230,6 @@
     <t>extra notes</t>
   </si>
   <si>
-    <t>DVR</t>
-  </si>
-  <si>
     <t>Sorbus aucuparia</t>
   </si>
   <si>
@@ -252,17 +245,201 @@
     <t>Fagus sylvatica</t>
   </si>
   <si>
-    <t>LT50</t>
-  </si>
-  <si>
-    <t>Lenz16, Lenz13</t>
+    <t>All plant functional types</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Eucalyptus pauciflora</t>
+  </si>
+  <si>
+    <t>natural</t>
+  </si>
+  <si>
+    <t>varying degress of damage across edges and interiors of forests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50% lethality </t>
+  </si>
+  <si>
+    <t>2 or more days at 2+ standard deviations below averge winter temperature</t>
+  </si>
+  <si>
+    <t>elevated CO2 study indicates higher levels of CO2 at same temperature cause greater damage to leaves</t>
+  </si>
+  <si>
+    <t>Lenz et al., 2016; Lenz et al., 2013</t>
+  </si>
+  <si>
+    <t>Barker et al., 2005</t>
+  </si>
+  <si>
+    <t>Vavrus et al., 2006</t>
+  </si>
+  <si>
+    <t>Augspurger, 2013</t>
+  </si>
+  <si>
+    <t>Schwartz, 1993</t>
+  </si>
+  <si>
+    <t>Date of spring onset - Last hard freeze date = damage index</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>barker05</t>
+  </si>
+  <si>
+    <t>lenz13</t>
+  </si>
+  <si>
+    <t>After budburst</t>
+  </si>
+  <si>
+    <t>Risk threshold</t>
+  </si>
+  <si>
+    <t>Cannell and Smith, 1986</t>
+  </si>
+  <si>
+    <t>tissue temperature can be 1-3 degrees lower on clear, still nights</t>
+  </si>
+  <si>
+    <t>Agricultural</t>
+  </si>
+  <si>
+    <t>damaging</t>
+  </si>
+  <si>
+    <t>Peterson and Abatzglou, 2014</t>
+  </si>
+  <si>
+    <t>use 7 day threshold between last freeze day after date of budburst as significant</t>
+  </si>
+  <si>
+    <t>2 SD below winter TAVG</t>
+  </si>
+  <si>
+    <t>Spring Onset</t>
+  </si>
+  <si>
+    <t>-4.4 to 0</t>
+  </si>
+  <si>
+    <t>Sprinkler protection threshold</t>
+  </si>
+  <si>
+    <t>Using sprinkler systems for blueberries in this temperature range can diminsh freeze damage</t>
+  </si>
+  <si>
+    <t>Longstroth, 2013</t>
+  </si>
+  <si>
+    <t>Vaccinium spp.</t>
+  </si>
+  <si>
+    <t>Flowers</t>
+  </si>
+  <si>
+    <t>Budburst to Leafout</t>
+  </si>
+  <si>
+    <t>Budburst</t>
+  </si>
+  <si>
+    <t>Rosaceae</t>
+  </si>
+  <si>
+    <t>10% lethality</t>
+  </si>
+  <si>
+    <t>experiment designed to measure specific temperature threshold by species</t>
+  </si>
+  <si>
+    <t>Longstroth, 2012</t>
+  </si>
+  <si>
+    <t>specifically apple and pear trees</t>
+  </si>
+  <si>
+    <t>90% lethality</t>
+  </si>
+  <si>
+    <t>All phenophases</t>
+  </si>
+  <si>
+    <t>Frost formation when temperature matches dew point</t>
+  </si>
+  <si>
+    <t>Occurs on calm, clear nights and boudary-layer inversion occurs</t>
+  </si>
+  <si>
+    <t>Radiation Frost</t>
+  </si>
+  <si>
+    <t>Barlow et al., 2015; Andresen, 2009</t>
+  </si>
+  <si>
+    <t>Wheat</t>
+  </si>
+  <si>
+    <t>-4 to -5</t>
+  </si>
+  <si>
+    <t>10%-90% lethality</t>
+  </si>
+  <si>
+    <r>
+      <t>if nighttime temperature drops by 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>℃, reaches 90% lethality</t>
+    </r>
+  </si>
+  <si>
+    <t>Barlow et al., 2015</t>
+  </si>
+  <si>
+    <t>Vegetative</t>
+  </si>
+  <si>
+    <t>100% lethality</t>
+  </si>
+  <si>
+    <t>-7 for 2hrs</t>
+  </si>
+  <si>
+    <t>From -4℃ to -7℃ during vegetative growth, 0-100% lethality</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>lethal limit</t>
+  </si>
+  <si>
+    <t>Sánchez et al., 2014</t>
+  </si>
+  <si>
+    <t>Corn</t>
+  </si>
+  <si>
+    <t>minimum temperature for 100% lethality</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -294,6 +471,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -312,7 +501,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -328,11 +517,49 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -340,6 +567,8 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -347,6 +576,8 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -614,7 +845,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -628,19 +859,19 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -648,7 +879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -656,7 +887,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -664,7 +895,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -672,12 +903,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -685,7 +916,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -693,7 +924,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -701,7 +932,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -709,15 +940,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -725,21 +956,16 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -751,13 +977,13 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -771,7 +997,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -785,7 +1011,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -799,7 +1025,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -813,7 +1039,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -827,7 +1053,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -840,25 +1066,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -875,226 +1096,565 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="D2" s="7">
+        <v>-7.4</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="7">
+        <v>-8.5</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="7">
+        <v>-7.4</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="7">
+        <v>-6.7</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="7">
+        <v>-4.8</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="7">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2">
-        <v>-7.4</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="7">
+        <v>-1.7</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="G8" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D3">
-        <v>-8.5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4">
-        <v>-7.4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D9" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D5">
-        <v>-6.7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D10" s="7">
+        <v>-5.8</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D6">
-        <v>-4.8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7">
+      <c r="F10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="7">
         <v>-2.2000000000000002</v>
       </c>
-      <c r="E7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E11" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8">
-        <v>-1.7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" t="s">
-        <v>58</v>
+      <c r="B12" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="7">
+        <v>2</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="7">
+        <v>-7.2</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="11">
+        <v>-13.3</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" s="7">
+        <v>4.7</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="7">
+        <v>-1.8</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="11">
+        <v>-17.2</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1106,34 +1666,29 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>